<commit_message>
Its devided by 1000 actually...
</commit_message>
<xml_diff>
--- a/task2.xlsx
+++ b/task2.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Реально достижимая</t>
   </si>
   <si>
-    <t xml:space="preserve">Млн. рублей</t>
+    <t xml:space="preserve">Млрд. рублей</t>
   </si>
   <si>
     <t xml:space="preserve">2028 год</t>
@@ -164,10 +164,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.97"/>

</xml_diff>